<commit_message>
Added comments and slight format modification. Added future improvements section.
</commit_message>
<xml_diff>
--- a/Workout.xlsx
+++ b/Workout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\PycharmProjects\pythonWeightCalculatorExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5382BF2E-67D0-45C0-8047-AFE36FF12157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CDA240-0FE0-48E6-859B-C48DCC09F4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16973" yWindow="-93" windowWidth="25787" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maxes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="79">
   <si>
     <t>Jesse</t>
   </si>
@@ -673,15 +673,15 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.26953125" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" customWidth="1"/>
     <col min="9" max="9" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -910,8 +910,8 @@
   </sheetPr>
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3178,17 +3178,114 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7265625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>0.95</v>
+      </c>
+      <c r="B3" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="B4" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>0.85</v>
+      </c>
+      <c r="B5" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="B6" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="B7" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="B8" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>0.65</v>
+      </c>
+      <c r="B9" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="B10" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B11" s="16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="B12" s="16">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated output cell locations and made more user friendly
</commit_message>
<xml_diff>
--- a/Workout.xlsx
+++ b/Workout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\PycharmProjects\pythonWeightCalculatorExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD45A40-12CE-4359-A9A4-73DE97D3D3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CCC4D7-9405-405F-AA4C-410BEF501496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16973" yWindow="-93" windowWidth="25787" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maxes" sheetId="1" r:id="rId1"/>
@@ -31,26 +31,16 @@
     <author>XX</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{15B3F878-634A-4F51-9436-E822B391B70B}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>XX:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">XX:
 Excluding the bar
 </t>
         </r>
@@ -61,7 +51,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="58">
+  <si>
+    <t>1 Rep Maxes</t>
+  </si>
   <si>
     <t>Percentage of 1RM</t>
   </si>
@@ -108,12 +101,30 @@
     <t>Total Weight</t>
   </si>
   <si>
+    <t>45.0, 5.0, 0.5</t>
+  </si>
+  <si>
+    <t>10.0, 5.0, 2.5, 0.75</t>
+  </si>
+  <si>
     <t>45.0, 10.0, 5.0, 2.5, 0.25</t>
   </si>
   <si>
+    <t>25.0, 5.0, 0.25</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 1.0</t>
+  </si>
+  <si>
+    <t>45.0, 10.0, 10.0, 2.5, 1.0, 0.5</t>
+  </si>
+  <si>
     <t>8+</t>
   </si>
   <si>
+    <t>45.0, 10.0, 1.0, 0.75</t>
+  </si>
+  <si>
     <t>Dumbell Isolation Curl</t>
   </si>
   <si>
@@ -126,9 +137,30 @@
     <t>Back Squat</t>
   </si>
   <si>
+    <t>45.0, 10.0, 2.5, 1.0, 0.75</t>
+  </si>
+  <si>
+    <t>45.0, 25.0, 5.0, 2.5, 1.0, 0.75, 0.25</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 10.0, 2.5, 0.75</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 5.0, 1.0, 0.5</t>
+  </si>
+  <si>
+    <t>45.0, 10.0, 10.0, 1.0</t>
+  </si>
+  <si>
     <t>Sumo Deadlift</t>
   </si>
   <si>
+    <t>45.0, 10.0, 1.0, 0.25</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 10.0, 10.0, 2.5, 1.0</t>
+  </si>
+  <si>
     <t>12+</t>
   </si>
   <si>
@@ -180,7 +212,10 @@
     <t>Front/Back Squat</t>
   </si>
   <si>
-    <t>User</t>
+    <t>45.0, 0.5</t>
+  </si>
+  <si>
+    <t>Weight Type</t>
   </si>
   <si>
     <t>Weight</t>
@@ -189,20 +224,14 @@
     <t>Quantity (in pairs)</t>
   </si>
   <si>
-    <t>Weight Type</t>
-  </si>
-  <si>
     <t>Bar</t>
-  </si>
-  <si>
-    <t>1 Rep Maxes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -253,19 +282,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="10"/>
@@ -275,7 +291,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +322,18 @@
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -328,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -352,8 +380,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +605,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -588,20 +618,20 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="9"/>
       <c r="F1" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="9">
         <v>245</v>
@@ -616,7 +646,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="9">
         <v>163</v>
@@ -632,7 +662,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="9">
         <v>145</v>
@@ -648,7 +678,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="9">
         <v>52.5</v>
@@ -664,7 +694,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="9">
         <v>35</v>
@@ -690,7 +720,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="9">
         <v>275</v>
@@ -705,7 +735,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="9">
         <v>320</v>
@@ -721,7 +751,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="9">
         <v>270</v>
@@ -758,7 +788,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -770,7 +800,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,45 +811,45 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="18"/>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="7"/>
       <c r="G2" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -835,7 +865,9 @@
       <c r="D3" s="8">
         <v>146.4</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="9">
         <v>1</v>
@@ -849,7 +881,9 @@
       <c r="J3" s="8">
         <v>81.5</v>
       </c>
-      <c r="K3" s="9"/>
+      <c r="K3" s="16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
@@ -864,7 +898,9 @@
       <c r="D4" s="8">
         <v>170.8</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="9">
         <v>2</v>
@@ -878,7 +914,9 @@
       <c r="J4" s="8">
         <v>105.95</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -894,7 +932,9 @@
       <c r="D5" s="8">
         <v>207.4</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="9">
         <v>3</v>
@@ -908,7 +948,9 @@
       <c r="J5" s="8">
         <v>105.95</v>
       </c>
-      <c r="K5" s="9"/>
+      <c r="K5" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -924,7 +966,9 @@
       <c r="D6" s="8">
         <v>207.4</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="9">
         <v>4</v>
@@ -937,6 +981,9 @@
       </c>
       <c r="J6" s="8">
         <v>105.95</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -952,7 +999,9 @@
       <c r="D7" s="8">
         <v>207.4</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="9">
         <v>5</v>
@@ -966,6 +1015,9 @@
       <c r="J7" s="8">
         <v>105.95</v>
       </c>
+      <c r="K7" s="15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
@@ -980,7 +1032,9 @@
       <c r="D8" s="8">
         <v>183</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="9">
         <v>6</v>
@@ -994,13 +1048,16 @@
       <c r="J8" s="8">
         <v>105.95</v>
       </c>
+      <c r="K8" s="15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C9" s="9">
         <v>0.65</v>
@@ -1008,47 +1065,49 @@
       <c r="D9" s="8">
         <v>158.6</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1098,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I14" s="9">
         <v>1</v>
@@ -1126,7 +1185,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I15" s="9">
         <v>1</v>
@@ -1154,7 +1213,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I16" s="9">
         <v>1</v>
@@ -1169,42 +1228,42 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1324,7 +1383,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1333,10 +1392,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1345,30 +1404,30 @@
     <col min="6" max="6" width="33.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -1378,11 +1437,14 @@
       <c r="C3" s="9">
         <v>0.6</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="20">
         <v>163.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -1392,11 +1454,14 @@
       <c r="C4" s="9">
         <v>0.75</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="20">
         <v>204.375</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -1406,11 +1471,14 @@
       <c r="C5" s="9">
         <v>0.85</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="20">
         <v>231.625</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -1420,11 +1488,14 @@
       <c r="C6" s="9">
         <v>0.85</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="20">
         <v>231.625</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -1434,11 +1505,14 @@
       <c r="C7" s="9">
         <v>0.85</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="20">
         <v>231.625</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -1448,48 +1522,54 @@
       <c r="C8" s="9">
         <v>0.8</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="20">
         <v>218</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C9" s="9">
         <v>0.65</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="20">
         <v>177.125</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>1</v>
       </c>
@@ -1499,11 +1579,14 @@
       <c r="C13" s="9">
         <v>0.5</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="20">
         <v>157.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>2</v>
       </c>
@@ -1513,11 +1596,14 @@
       <c r="C14" s="9">
         <v>0.8</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="20">
         <v>252</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>3</v>
       </c>
@@ -1527,11 +1613,14 @@
       <c r="C15" s="9">
         <v>0.8</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="20">
         <v>252</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>4</v>
       </c>
@@ -1541,25 +1630,28 @@
       <c r="C16" s="9">
         <v>0.8</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="20">
         <v>252</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1567,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C22" s="9">
         <v>218</v>
@@ -1578,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C23" s="9">
         <v>218</v>
@@ -1589,7 +1681,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C24" s="9">
         <v>218</v>
@@ -1600,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C25" s="9">
         <v>218</v>
@@ -1608,32 +1700,32 @@
     </row>
     <row r="33" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1658,50 +1750,50 @@
     <col min="7" max="7" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2"/>
       <c r="G1" s="9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -1715,17 +1807,17 @@
         <v>145</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9">
         <v>1</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="J3" s="9">
         <v>1</v>
@@ -1735,12 +1827,12 @@
       </c>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C4" s="9">
         <v>0.7</v>
@@ -1749,7 +1841,7 @@
         <v>170.8</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G4" s="9">
         <v>2</v>
@@ -1758,7 +1850,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="J4" s="9">
         <v>1</v>
@@ -1768,12 +1860,12 @@
       </c>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C5" s="9">
         <v>0.7</v>
@@ -1782,7 +1874,7 @@
         <v>170.8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9">
@@ -1792,7 +1884,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="J5" s="9">
         <v>1</v>
@@ -1802,12 +1894,12 @@
       </c>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C6" s="9">
         <v>0.7</v>
@@ -1816,7 +1908,7 @@
         <v>170.8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G6" s="9">
         <v>4</v>
@@ -1825,7 +1917,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="J6" s="9">
         <v>1</v>
@@ -1835,12 +1927,12 @@
       </c>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9">
         <v>0.7</v>
@@ -1849,50 +1941,50 @@
         <v>170.8</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2"/>
       <c r="G9" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="9">
         <v>1</v>
@@ -1908,7 +2000,7 @@
       </c>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>1</v>
       </c>
@@ -1922,7 +2014,7 @@
         <v>145</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G11" s="9">
         <v>2</v>
@@ -1938,7 +2030,7 @@
       </c>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>2</v>
       </c>
@@ -1952,7 +2044,7 @@
         <v>145</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G12" s="9">
         <v>3</v>
@@ -1968,7 +2060,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>3</v>
       </c>
@@ -1982,7 +2074,7 @@
         <v>145</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G13" s="9">
         <v>4</v>
@@ -1998,7 +2090,7 @@
       </c>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>4</v>
       </c>
@@ -2012,47 +2104,47 @@
         <v>145</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2"/>
       <c r="G16" s="9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" s="7"/>
       <c r="G17" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>1</v>
       </c>
@@ -2079,7 +2171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>2</v>
       </c>
@@ -2097,7 +2189,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I19" s="9">
         <v>1</v>
@@ -2106,7 +2198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>3</v>
       </c>
@@ -2124,7 +2216,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I20" s="9">
         <v>1</v>
@@ -2150,7 +2242,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I21" s="9">
         <v>1</v>
@@ -2159,7 +2251,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F43" s="7"/>
     </row>
   </sheetData>
@@ -2175,7 +2267,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2185,27 +2277,25 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2222,7 +2312,7 @@
         <v>212.625</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F3" s="15"/>
     </row>
@@ -2240,7 +2330,7 @@
         <v>236.25</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="F4" s="15"/>
     </row>
@@ -2249,7 +2339,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9">
         <v>0.875</v>
@@ -2258,7 +2348,7 @@
         <v>275.625</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F5" s="15"/>
     </row>
@@ -2267,7 +2357,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C6" s="9">
         <v>0.875</v>
@@ -2276,7 +2366,7 @@
         <v>275.625</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -2285,7 +2375,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C7" s="9">
         <v>0.875</v>
@@ -2294,7 +2384,7 @@
         <v>275.625</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F7" s="15"/>
     </row>
@@ -2302,35 +2392,33 @@
     <row r="9" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>1</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C12" s="9">
         <v>0.5</v>
@@ -2338,13 +2426,16 @@
       <c r="D12" s="9">
         <v>136.25</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>2</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C13" s="9">
         <v>0.5</v>
@@ -2352,13 +2443,16 @@
       <c r="D13" s="9">
         <v>136.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>3</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C14" s="9">
         <v>0.5</v>
@@ -2366,13 +2460,16 @@
       <c r="D14" s="9">
         <v>136.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>4</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9">
         <v>0.5</v>
@@ -2380,13 +2477,16 @@
       <c r="D15" s="9">
         <v>136.25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>5</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C16" s="9">
         <v>0.5</v>
@@ -2394,13 +2494,16 @@
       <c r="D16" s="9">
         <v>136.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>6</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C17" s="9">
         <v>0.5</v>
@@ -2408,60 +2511,61 @@
       <c r="D17" s="9">
         <v>136.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>1</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>2</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>3</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>4</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2488,10 +2592,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2588,7 +2692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6A0ABB-B9DE-4A4F-865D-7703F45C5BAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2602,18 +2706,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>45</v>

</xml_diff>

<commit_message>
Moved all program logic into Python and created update_total() function
</commit_message>
<xml_diff>
--- a/Workout.xlsx
+++ b/Workout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\PycharmProjects\pythonWeightCalculatorExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1770D39-4C40-470D-84B1-76C69BCF1070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA9B27D-5659-4C75-843E-F2E5A15ACF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,7 @@
     <sheet name="Lower1" sheetId="3" r:id="rId3"/>
     <sheet name="Upper2" sheetId="4" r:id="rId4"/>
     <sheet name="Lower2" sheetId="5" r:id="rId5"/>
-    <sheet name="Theoretical Weight Scheme" sheetId="6" r:id="rId6"/>
-    <sheet name="Weights" sheetId="7" r:id="rId7"/>
+    <sheet name="Weights" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -31,7 +30,7 @@
     <author>XX</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="52">
   <si>
     <t>1 Rep Maxes</t>
   </si>
@@ -71,18 +70,18 @@
     <t>Barbell Row</t>
   </si>
   <si>
+    <t>Squat</t>
+  </si>
+  <si>
+    <t>Deadlift</t>
+  </si>
+  <si>
+    <t>Calf Raise</t>
+  </si>
+  <si>
     <t>Isolation Curl</t>
   </si>
   <si>
-    <t>Squat</t>
-  </si>
-  <si>
-    <t>Deadlift</t>
-  </si>
-  <si>
-    <t>Calf Raise</t>
-  </si>
-  <si>
     <t>Primary</t>
   </si>
   <si>
@@ -104,19 +103,19 @@
     <t>Output</t>
   </si>
   <si>
-    <t>45.0, 5.0, 0.5</t>
-  </si>
-  <si>
-    <t>45.0, 10.0, 5.0, 2.5, 0.25</t>
+    <t>45.0, 5.0, 2.5</t>
+  </si>
+  <si>
+    <t>45.0, 10.0, 10.0</t>
   </si>
   <si>
     <t>8 to 12</t>
   </si>
   <si>
-    <t>45.0, 35.0, 1.0</t>
-  </si>
-  <si>
-    <t>45.0, 10.0, 10.0, 2.5, 1.0, 0.5</t>
+    <t>45.0, 35.0, 2.5, 1.0, 0.25</t>
+  </si>
+  <si>
+    <t>45.0, 25.0, 1.0, 0.25</t>
   </si>
   <si>
     <t>Pull-Ups</t>
@@ -125,70 +124,52 @@
     <t>8+</t>
   </si>
   <si>
-    <t>45.0, 10.0, 1.0, 0.75</t>
-  </si>
-  <si>
-    <t>10.0, 5.0, 2.5, 0.75</t>
-  </si>
-  <si>
-    <t>25.0, 5.0, 0.25</t>
-  </si>
-  <si>
-    <t>45.0, 5.0</t>
+    <t>45.0, 10.0, 2.5, 1.0, 0.25</t>
+  </si>
+  <si>
+    <t>10.0, 5.0, 2.5, 1.0, 0.25</t>
+  </si>
+  <si>
+    <t>25.0, 5.0, 1.0</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>45.0, 10.0</t>
   </si>
   <si>
     <t>Back Squat</t>
   </si>
   <si>
-    <t>45.0, 10.0, 2.5, 1.0, 0.75</t>
-  </si>
-  <si>
-    <t>45.0, 25.0, 5.0, 2.5, 1.0, 0.75, 0.25</t>
-  </si>
-  <si>
-    <t>45.0, 35.0, 10.0, 2.5, 0.75</t>
-  </si>
-  <si>
-    <t>45.0, 35.0, 5.0, 1.0, 0.5</t>
-  </si>
-  <si>
-    <t>45.0, 10.0, 10.0, 1.0</t>
+    <t>45.0, 10.0, 5.0</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 0.5</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 10.0, 2.5, 1.0, 0.75</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 5.0, 2.5</t>
+  </si>
+  <si>
+    <t>45.0, 10.0, 10.0, 1.0, 0.75</t>
   </si>
   <si>
     <t>Sumo Deadlift</t>
   </si>
   <si>
-    <t>45.0, 10.0, 1.0, 0.25</t>
-  </si>
-  <si>
-    <t>45.0, 35.0, 10.0, 10.0, 2.5, 1.0</t>
-  </si>
-  <si>
-    <t>Secondary</t>
+    <t>45.0, 10.0, 2.5</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 25.0, 0.5</t>
   </si>
   <si>
     <t>12+</t>
   </si>
   <si>
-    <t>45.0, 35.0, 5.0</t>
-  </si>
-  <si>
-    <t>Warm-Up Routine</t>
-  </si>
-  <si>
-    <t>Single Leg Squat on Stairs</t>
-  </si>
-  <si>
-    <t>Hip Internal Rotation</t>
-  </si>
-  <si>
-    <t>Hip External Rotation</t>
-  </si>
-  <si>
-    <t>Ankle Mobilization (forward)</t>
-  </si>
-  <si>
-    <t>Ankle Mobilization (lateral)</t>
+    <t>45.0, 35.0, 25.0, 5.0, 2.5</t>
   </si>
   <si>
     <t>12 to 15</t>
@@ -200,22 +181,19 @@
     <t>Close-grip Bench Press</t>
   </si>
   <si>
-    <t>45.0, 35.0, 2.5, 1.0, 0.25</t>
-  </si>
-  <si>
-    <t>45.0, 35.0, 10.0, 5.0, 0.5</t>
+    <t>45.0, 35.0, 5.0, 0.5</t>
+  </si>
+  <si>
+    <t>45.0, 35.0, 10.0, 5.0, 2.5</t>
   </si>
   <si>
     <t>3 to 4</t>
   </si>
   <si>
-    <t>45.0, 35.0, 25.0, 10.0, 0.25</t>
-  </si>
-  <si>
-    <t>Front/Back Squat</t>
-  </si>
-  <si>
-    <t>45.0, 0.5</t>
+    <t>45.0, 35.0, 25.0, 10.0, 2.5</t>
+  </si>
+  <si>
+    <t>Front Squat</t>
   </si>
   <si>
     <t>Weight Type</t>
@@ -613,34 +591,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J8" sqref="J7:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" customWidth="1"/>
     <col min="6" max="6" width="17.36328125" customWidth="1"/>
     <col min="9" max="9" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="F1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -648,14 +626,14 @@
         <v>250</v>
       </c>
       <c r="C2" s="9"/>
-      <c r="F2" s="9">
-        <v>1</v>
-      </c>
-      <c r="G2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -663,15 +641,14 @@
         <v>165</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="F3" s="9">
+      <c r="D3" s="9">
         <v>0.95</v>
       </c>
-      <c r="G3" s="9">
+      <c r="E3" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -679,114 +656,106 @@
         <v>155</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="F4" s="9">
+      <c r="D4" s="9">
         <v>0.9</v>
       </c>
-      <c r="G4" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="9">
+        <v>275</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="E5" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9">
+        <v>320</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9">
+        <v>270</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9">
         <v>35</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="F5" s="9">
-        <v>0.85</v>
-      </c>
-      <c r="G5" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="F6" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="G6" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="9">
-        <v>275</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="F7" s="9">
-        <v>0.75</v>
-      </c>
-      <c r="G7" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9">
-        <v>320</v>
-      </c>
       <c r="C8" s="9"/>
-      <c r="F8" s="9">
+      <c r="D8" s="9">
         <v>0.7</v>
       </c>
-      <c r="G8" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="9">
-        <v>270</v>
-      </c>
+      <c r="E8" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="F9" s="9">
+      <c r="D9" s="9">
         <v>0.65</v>
       </c>
-      <c r="G9" s="9">
+      <c r="E9" s="9">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="F10" s="9">
+      <c r="D10" s="9">
         <v>0.6</v>
       </c>
-      <c r="G10" s="9">
+      <c r="E10" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="F11" s="9">
+      <c r="D11" s="9">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G11" s="9">
+      <c r="E11" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="9"/>
-      <c r="F12" s="9">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="9">
         <v>0.5</v>
       </c>
-      <c r="G12" s="9">
+      <c r="E12" s="9">
         <v>30</v>
       </c>
     </row>
@@ -804,7 +773,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -866,7 +835,7 @@
         <v>0.6</v>
       </c>
       <c r="D3" s="8">
-        <v>146.4</v>
+        <v>150</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>17</v>
@@ -897,7 +866,7 @@
         <v>0.7</v>
       </c>
       <c r="D4" s="8">
-        <v>170.8</v>
+        <v>175</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>18</v>
@@ -929,7 +898,7 @@
         <v>0.85</v>
       </c>
       <c r="D5" s="8">
-        <v>207.4</v>
+        <v>212.5</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>20</v>
@@ -961,7 +930,7 @@
         <v>0.85</v>
       </c>
       <c r="D6" s="8">
-        <v>207.4</v>
+        <v>212.5</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>20</v>
@@ -991,7 +960,7 @@
         <v>0.85</v>
       </c>
       <c r="D7" s="8">
-        <v>207.4</v>
+        <v>212.5</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>20</v>
@@ -1010,7 +979,7 @@
         <v>0.75</v>
       </c>
       <c r="D8" s="8">
-        <v>183</v>
+        <v>187.5</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>21</v>
@@ -1033,7 +1002,7 @@
         <v>0.65</v>
       </c>
       <c r="D9" s="8">
-        <v>158.6</v>
+        <v>162.5</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>24</v>
@@ -1128,7 +1097,7 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="8">
-        <v>81.5</v>
+        <v>82.5</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>25</v>
@@ -1158,7 +1127,7 @@
         <v>0.65</v>
       </c>
       <c r="D14" s="8">
-        <v>105.95</v>
+        <v>107.25</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>26</v>
@@ -1176,7 +1145,7 @@
         <v>0.65</v>
       </c>
       <c r="D15" s="8">
-        <v>105.95</v>
+        <v>107.25</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>26</v>
@@ -1194,7 +1163,7 @@
         <v>0.65</v>
       </c>
       <c r="D16" s="8">
-        <v>105.95</v>
+        <v>107.25</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>26</v>
@@ -1212,7 +1181,7 @@
         <v>0.65</v>
       </c>
       <c r="D17" s="8">
-        <v>105.95</v>
+        <v>107.25</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>26</v>
@@ -1230,7 +1199,7 @@
         <v>0.65</v>
       </c>
       <c r="D18" s="8">
-        <v>105.95</v>
+        <v>107.25</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>26</v>
@@ -1246,7 +1215,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="7"/>
@@ -1279,10 +1248,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="8">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" s="7"/>
     </row>
@@ -1297,10 +1266,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="8">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F23" s="7"/>
     </row>
@@ -1315,10 +1284,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="8">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1332,10 +1301,10 @@
         <v>1</v>
       </c>
       <c r="D25" s="8">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1356,7 +1325,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1336,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>10</v>
@@ -1402,10 +1371,10 @@
         <v>0.6</v>
       </c>
       <c r="D3" s="20">
-        <v>163.5</v>
+        <v>165</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1419,10 +1388,10 @@
         <v>0.75</v>
       </c>
       <c r="D4" s="20">
-        <v>204.375</v>
+        <v>206.25</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1436,10 +1405,10 @@
         <v>0.85</v>
       </c>
       <c r="D5" s="20">
-        <v>231.625</v>
+        <v>233.75</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1453,10 +1422,10 @@
         <v>0.85</v>
       </c>
       <c r="D6" s="20">
-        <v>231.625</v>
+        <v>233.75</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1470,10 +1439,10 @@
         <v>0.85</v>
       </c>
       <c r="D7" s="20">
-        <v>231.625</v>
+        <v>233.75</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1487,10 +1456,10 @@
         <v>0.8</v>
       </c>
       <c r="D8" s="20">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1504,10 +1473,10 @@
         <v>0.65</v>
       </c>
       <c r="D9" s="20">
-        <v>177.125</v>
+        <v>178.75</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1515,7 +1484,7 @@
     </row>
     <row r="11" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>10</v>
@@ -1549,10 +1518,10 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="20">
-        <v>157.5</v>
+        <v>160</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1566,10 +1535,10 @@
         <v>0.8</v>
       </c>
       <c r="D14" s="20">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1583,10 +1552,10 @@
         <v>0.8</v>
       </c>
       <c r="D15" s="20">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1600,10 +1569,10 @@
         <v>0.8</v>
       </c>
       <c r="D16" s="20">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1617,10 +1586,10 @@
     </row>
     <row r="20" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="15"/>
@@ -1651,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="20">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>39</v>
@@ -1668,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="20">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>39</v>
@@ -1685,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="20">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>39</v>
@@ -1702,45 +1671,33 @@
         <v>1</v>
       </c>
       <c r="D25" s="20">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="A33" s="9"/>
     </row>
     <row r="34" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>41</v>
-      </c>
+      <c r="A34" s="9"/>
     </row>
     <row r="35" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A35" s="9"/>
     </row>
     <row r="36" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A36" s="9"/>
     </row>
     <row r="37" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="A37" s="9"/>
     </row>
     <row r="38" spans="1:1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="A38" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1752,7 +1709,7 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1818,20 +1775,20 @@
         <v>0.6</v>
       </c>
       <c r="D3" s="12">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9">
         <v>1</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J3" s="9">
         <v>1</v>
@@ -1852,7 +1809,7 @@
         <v>0.7</v>
       </c>
       <c r="D4" s="12">
-        <v>170.8</v>
+        <v>175</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>18</v>
@@ -1864,7 +1821,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J4" s="9">
         <v>1</v>
@@ -1885,7 +1842,7 @@
         <v>0.7</v>
       </c>
       <c r="D5" s="12">
-        <v>170.8</v>
+        <v>175</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>18</v>
@@ -1898,7 +1855,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J5" s="9">
         <v>1</v>
@@ -1919,7 +1876,7 @@
         <v>0.7</v>
       </c>
       <c r="D6" s="12">
-        <v>170.8</v>
+        <v>175</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>18</v>
@@ -1931,7 +1888,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J6" s="9">
         <v>1</v>
@@ -1952,7 +1909,7 @@
         <v>0.7</v>
       </c>
       <c r="D7" s="12">
-        <v>170.8</v>
+        <v>175</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>18</v>
@@ -1967,10 +1924,10 @@
     </row>
     <row r="9" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2"/>
       <c r="G9" s="9" t="s">
@@ -2025,10 +1982,10 @@
         <v>0.6</v>
       </c>
       <c r="D11" s="12">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G11" s="9">
         <v>2</v>
@@ -2055,10 +2012,10 @@
         <v>0.6</v>
       </c>
       <c r="D12" s="12">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G12" s="9">
         <v>3</v>
@@ -2085,10 +2042,10 @@
         <v>0.6</v>
       </c>
       <c r="D13" s="12">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G13" s="9">
         <v>4</v>
@@ -2115,10 +2072,10 @@
         <v>0.6</v>
       </c>
       <c r="D14" s="12">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -2153,10 +2110,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="12">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -2170,10 +2127,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="12">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -2187,10 +2144,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="12">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2204,10 +2161,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="12">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="6:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -2226,7 +2183,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G9" sqref="G9:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2236,7 +2193,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>10</v>
@@ -2271,10 +2228,10 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="D3" s="9">
-        <v>212.625</v>
+        <v>216</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F3" s="15"/>
     </row>
@@ -2289,10 +2246,10 @@
         <v>0.75</v>
       </c>
       <c r="D4" s="9">
-        <v>236.25</v>
+        <v>240</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F4" s="15"/>
     </row>
@@ -2301,16 +2258,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C5" s="9">
         <v>0.875</v>
       </c>
       <c r="D5" s="9">
-        <v>275.625</v>
+        <v>280</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F5" s="15"/>
     </row>
@@ -2319,16 +2276,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C6" s="9">
         <v>0.875</v>
       </c>
       <c r="D6" s="9">
-        <v>275.625</v>
+        <v>280</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -2337,16 +2294,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C7" s="9">
         <v>0.875</v>
       </c>
       <c r="D7" s="9">
-        <v>275.625</v>
+        <v>280</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F7" s="15"/>
     </row>
@@ -2354,7 +2311,7 @@
     <row r="9" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>10</v>
@@ -2379,102 +2336,102 @@
       <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>19</v>
+      <c r="B12" s="9">
+        <v>6</v>
       </c>
       <c r="C12" s="9">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D12" s="9">
-        <v>136.25</v>
+        <v>165</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>2</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>19</v>
+      <c r="B13" s="9">
+        <v>6</v>
       </c>
       <c r="C13" s="9">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D13" s="9">
-        <v>136.25</v>
+        <v>165</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>3</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>19</v>
+      <c r="B14" s="9">
+        <v>6</v>
       </c>
       <c r="C14" s="9">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D14" s="9">
-        <v>136.25</v>
+        <v>165</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>4</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>19</v>
+      <c r="B15" s="9">
+        <v>6</v>
       </c>
       <c r="C15" s="9">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D15" s="9">
-        <v>136.25</v>
+        <v>165</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>5</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>19</v>
+      <c r="B16" s="9">
+        <v>6</v>
       </c>
       <c r="C16" s="9">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D16" s="9">
-        <v>136.25</v>
+        <v>165</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>6</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>19</v>
+      <c r="B17" s="9">
+        <v>6</v>
       </c>
       <c r="C17" s="9">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D17" s="9">
-        <v>136.25</v>
+        <v>165</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2483,10 +2440,10 @@
     </row>
     <row r="19" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -2515,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>39</v>
@@ -2532,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>39</v>
@@ -2549,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>39</v>
@@ -2566,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>39</v>
@@ -2582,128 +2539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>0.95</v>
-      </c>
-      <c r="B3" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="B4" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>0.85</v>
-      </c>
-      <c r="B5" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="B6" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>0.75</v>
-      </c>
-      <c r="B7" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="B8" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>0.65</v>
-      </c>
-      <c r="B9" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="B10" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="B11" s="9">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="B12" s="9">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2713,18 +2553,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B2">
         <v>45</v>

</xml_diff>